<commit_message>
Enable development mode in the remaining files
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_TRA_12TimeSlices.xlsx
+++ b/SuppXLS/Scen_TRA_12TimeSlices.xlsx
@@ -8,22 +8,41 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88788855-B512-43AA-86C2-AC460D257C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C143C422-0731-4879-9C51-E04ED9592FDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6165" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="INS" sheetId="2" r:id="rId1"/>
-    <sheet name="UPD" sheetId="11" r:id="rId2"/>
-    <sheet name="UCT1" sheetId="1" r:id="rId3"/>
-    <sheet name="UCT2" sheetId="12" r:id="rId4"/>
-    <sheet name="UCT3" sheetId="13" r:id="rId5"/>
-    <sheet name="UCT4" sheetId="14" r:id="rId6"/>
-    <sheet name="Sheet6" sheetId="6" r:id="rId7"/>
+    <sheet name="Regions" sheetId="15" r:id="rId1"/>
+    <sheet name="INS" sheetId="2" r:id="rId2"/>
+    <sheet name="UPD" sheetId="11" r:id="rId3"/>
+    <sheet name="UCT1" sheetId="1" r:id="rId4"/>
+    <sheet name="UCT2" sheetId="12" r:id="rId5"/>
+    <sheet name="UCT3" sheetId="13" r:id="rId6"/>
+    <sheet name="UCT4" sheetId="14" r:id="rId7"/>
+    <sheet name="COM_FR" sheetId="6" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
+    <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
+    <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -60,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="AJ2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="AO2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -96,7 +115,7 @@
     <author>Gary Goldstein</author>
   </authors>
   <commentList>
-    <comment ref="AI2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="AJ2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -109,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="AO2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -160,8 +179,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="153">
   <si>
     <t>~UC_Sets: R_E: AllRegions</t>
   </si>
@@ -440,13 +481,213 @@
   </si>
   <si>
     <t>Load curves</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>National</t>
+  </si>
+  <si>
+    <t>Single-region</t>
+  </si>
+  <si>
+    <t>Multi-region</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>County name</t>
+  </si>
+  <si>
+    <t>IE-CW</t>
+  </si>
+  <si>
+    <t>Carlow</t>
+  </si>
+  <si>
+    <t>IE-CN</t>
+  </si>
+  <si>
+    <t>Cavan</t>
+  </si>
+  <si>
+    <t>IE-CE</t>
+  </si>
+  <si>
+    <t>Clare</t>
+  </si>
+  <si>
+    <t>IE-CO</t>
+  </si>
+  <si>
+    <t>Cork</t>
+  </si>
+  <si>
+    <t>IE-DL</t>
+  </si>
+  <si>
+    <t>Donegal</t>
+  </si>
+  <si>
+    <t>IE-D</t>
+  </si>
+  <si>
+    <t>Dublin</t>
+  </si>
+  <si>
+    <t>IE-G</t>
+  </si>
+  <si>
+    <t>Galway</t>
+  </si>
+  <si>
+    <t>IE-KY</t>
+  </si>
+  <si>
+    <t>Kerry</t>
+  </si>
+  <si>
+    <t>IE-KE</t>
+  </si>
+  <si>
+    <t>Kildare</t>
+  </si>
+  <si>
+    <t>IE-KK</t>
+  </si>
+  <si>
+    <t>Kilkenny</t>
+  </si>
+  <si>
+    <t>IE-LS</t>
+  </si>
+  <si>
+    <t>Laois</t>
+  </si>
+  <si>
+    <t>IE-LM</t>
+  </si>
+  <si>
+    <t>Leitrim</t>
+  </si>
+  <si>
+    <t>IE-LK</t>
+  </si>
+  <si>
+    <t>Limerick</t>
+  </si>
+  <si>
+    <t>IE-LD</t>
+  </si>
+  <si>
+    <t>Longford</t>
+  </si>
+  <si>
+    <t>IE-LH</t>
+  </si>
+  <si>
+    <t>Louth</t>
+  </si>
+  <si>
+    <t>IE-MO</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>IE-MH</t>
+  </si>
+  <si>
+    <t>Meath</t>
+  </si>
+  <si>
+    <t>IE-MN</t>
+  </si>
+  <si>
+    <t>Monaghan</t>
+  </si>
+  <si>
+    <t>IE-OY</t>
+  </si>
+  <si>
+    <t>Offaly</t>
+  </si>
+  <si>
+    <t>IE-RN</t>
+  </si>
+  <si>
+    <t>Roscommon</t>
+  </si>
+  <si>
+    <t>IE-SO</t>
+  </si>
+  <si>
+    <t>Sligo</t>
+  </si>
+  <si>
+    <t>IE-TA</t>
+  </si>
+  <si>
+    <t>Tipperary</t>
+  </si>
+  <si>
+    <t>IE-WD</t>
+  </si>
+  <si>
+    <t>Waterford</t>
+  </si>
+  <si>
+    <t>IE-WH</t>
+  </si>
+  <si>
+    <t>Westmeath</t>
+  </si>
+  <si>
+    <t>IE-WX</t>
+  </si>
+  <si>
+    <t>Wexford</t>
+  </si>
+  <si>
+    <t>IE-WW</t>
+  </si>
+  <si>
+    <t>Wicklow</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Source: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://en.wikipedia.org/wiki/ISO_3166-2:IE</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,19 +708,98 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -488,8 +808,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,124 +838,95 @@
 </styleSheet>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Drop" dropStyle="combo" dx="39" fmlaLink="$A$4" fmlaRange="$A$5:$A$7" noThreeD="1" sel="1" val="0"/>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>1</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5121" name="Drop Down 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s5121"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A365913-E6A6-48A3-8F48-B6BCCDFAB5E5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Intro"/>
-      <sheetName val="Notes"/>
-      <sheetName val="EB2018"/>
       <sheetName val="Regions"/>
-      <sheetName val="Primary"/>
-      <sheetName val="Secondary"/>
-      <sheetName val="Commodities"/>
-      <sheetName val="Stock"/>
-      <sheetName val="Demands"/>
-      <sheetName val="On-Road Fac."/>
-      <sheetName val="ACT2FLO"/>
-      <sheetName val="Efficiency"/>
-      <sheetName val="AF"/>
+      <sheetName val="INS"/>
+      <sheetName val="UPD"/>
+      <sheetName val="UCT1"/>
+      <sheetName val="UCT2"/>
+      <sheetName val="UCT3"/>
+      <sheetName val="UCT4"/>
+      <sheetName val="COM_PROJ"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3"/>
-      <sheetData sheetId="4">
-        <row r="2">
-          <cell r="B2" t="str">
-            <v>*National</v>
-          </cell>
-          <cell r="C2" t="str">
-            <v>IE-CW</v>
-          </cell>
-          <cell r="D2" t="str">
-            <v>IE-D</v>
-          </cell>
-          <cell r="E2" t="str">
-            <v>IE-KE</v>
-          </cell>
-          <cell r="F2" t="str">
-            <v>IE-KK</v>
-          </cell>
-          <cell r="G2" t="str">
-            <v>IE-LS</v>
-          </cell>
-          <cell r="H2" t="str">
-            <v>IE-LD</v>
-          </cell>
-          <cell r="I2" t="str">
-            <v>IE-LH</v>
-          </cell>
-          <cell r="J2" t="str">
-            <v>IE-MH</v>
-          </cell>
-          <cell r="K2" t="str">
-            <v>IE-OY</v>
-          </cell>
-          <cell r="L2" t="str">
-            <v>IE-WH</v>
-          </cell>
-          <cell r="M2" t="str">
-            <v>IE-WX</v>
-          </cell>
-          <cell r="N2" t="str">
-            <v>IE-WW</v>
-          </cell>
-          <cell r="O2" t="str">
-            <v>IE-CE</v>
-          </cell>
-          <cell r="P2" t="str">
-            <v>IE-CO</v>
-          </cell>
-          <cell r="Q2" t="str">
-            <v>IE-KY</v>
-          </cell>
-          <cell r="R2" t="str">
-            <v>IE-LK</v>
-          </cell>
-          <cell r="S2" t="str">
-            <v>IE-TA</v>
-          </cell>
-          <cell r="T2" t="str">
-            <v>IE-WD</v>
-          </cell>
-          <cell r="U2" t="str">
-            <v>IE-G</v>
-          </cell>
-          <cell r="V2" t="str">
-            <v>IE-LM</v>
-          </cell>
-          <cell r="W2" t="str">
-            <v>IE-MO</v>
-          </cell>
-          <cell r="X2" t="str">
-            <v>IE-RN</v>
-          </cell>
-          <cell r="Y2" t="str">
-            <v>IE-SO</v>
-          </cell>
-          <cell r="Z2" t="str">
-            <v>IE-CN</v>
-          </cell>
-          <cell r="AA2" t="str">
-            <v>IE-DL</v>
-          </cell>
-          <cell r="AB2" t="str">
-            <v>IE-MN</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -950,12 +1252,777 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346B1C79-67D0-4788-9E2B-7EDF4F915007}">
+  <dimension ref="A3:AD37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.53125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.46484375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.9296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.46484375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.06640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.53125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.19921875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.06640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.9296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.53125" customWidth="1"/>
+    <col min="25" max="25" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.06640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="C3" s="1" t="str" cm="1">
+        <f t="array" ref="C3">INDEX(C5:C7,$A$4)</f>
+        <v>IE</v>
+      </c>
+      <c r="D3" s="1" t="str" cm="1">
+        <f t="array" ref="D3">INDEX(D5:D7,$A$4)</f>
+        <v>National</v>
+      </c>
+      <c r="E3" s="1" t="str" cm="1">
+        <f t="array" ref="E3">INDEX(E5:E7,$A$4)</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="F3" s="1" t="str" cm="1">
+        <f t="array" ref="F3">INDEX(F5:F7,$A$4)</f>
+        <v>IE-D</v>
+      </c>
+      <c r="G3" s="1" t="str" cm="1">
+        <f t="array" ref="G3">INDEX(G5:G7,$A$4)</f>
+        <v>IE-KE</v>
+      </c>
+      <c r="H3" s="1" t="str" cm="1">
+        <f t="array" ref="H3">INDEX(H5:H7,$A$4)</f>
+        <v>IE-KK</v>
+      </c>
+      <c r="I3" s="1" t="str" cm="1">
+        <f t="array" ref="I3">INDEX(I5:I7,$A$4)</f>
+        <v>IE-LS</v>
+      </c>
+      <c r="J3" s="1" t="str" cm="1">
+        <f t="array" ref="J3">INDEX(J5:J7,$A$4)</f>
+        <v>IE-LD</v>
+      </c>
+      <c r="K3" s="1" t="str" cm="1">
+        <f t="array" ref="K3">INDEX(K5:K7,$A$4)</f>
+        <v>IE-LH</v>
+      </c>
+      <c r="L3" s="1" t="str" cm="1">
+        <f t="array" ref="L3">INDEX(L5:L7,$A$4)</f>
+        <v>IE-MH</v>
+      </c>
+      <c r="M3" s="1" t="str" cm="1">
+        <f t="array" ref="M3">INDEX(M5:M7,$A$4)</f>
+        <v>IE-OY</v>
+      </c>
+      <c r="N3" s="1" t="str" cm="1">
+        <f t="array" ref="N3">INDEX(N5:N7,$A$4)</f>
+        <v>IE-WH</v>
+      </c>
+      <c r="O3" s="1" t="str" cm="1">
+        <f t="array" ref="O3">INDEX(O5:O7,$A$4)</f>
+        <v>IE-WX</v>
+      </c>
+      <c r="P3" s="1" t="str" cm="1">
+        <f t="array" ref="P3">INDEX(P5:P7,$A$4)</f>
+        <v>IE-WW</v>
+      </c>
+      <c r="Q3" s="1" t="str" cm="1">
+        <f t="array" ref="Q3">INDEX(Q5:Q7,$A$4)</f>
+        <v>IE-CE</v>
+      </c>
+      <c r="R3" s="1" t="str" cm="1">
+        <f t="array" ref="R3">INDEX(R5:R7,$A$4)</f>
+        <v>IE-CO</v>
+      </c>
+      <c r="S3" s="1" t="str" cm="1">
+        <f t="array" ref="S3">INDEX(S5:S7,$A$4)</f>
+        <v>IE-KY</v>
+      </c>
+      <c r="T3" s="1" t="str" cm="1">
+        <f t="array" ref="T3">INDEX(T5:T7,$A$4)</f>
+        <v>IE-LK</v>
+      </c>
+      <c r="U3" s="1" t="str" cm="1">
+        <f t="array" ref="U3">INDEX(U5:U7,$A$4)</f>
+        <v>IE-TA</v>
+      </c>
+      <c r="V3" s="1" t="str" cm="1">
+        <f t="array" ref="V3">INDEX(V5:V7,$A$4)</f>
+        <v>IE-WD</v>
+      </c>
+      <c r="W3" s="1" t="str" cm="1">
+        <f t="array" ref="W3">INDEX(W5:W7,$A$4)</f>
+        <v>IE-G</v>
+      </c>
+      <c r="X3" s="1" t="str" cm="1">
+        <f t="array" ref="X3">INDEX(X5:X7,$A$4)</f>
+        <v>IE-LM</v>
+      </c>
+      <c r="Y3" s="1" t="str" cm="1">
+        <f t="array" ref="Y3">INDEX(Y5:Y7,$A$4)</f>
+        <v>IE-MO</v>
+      </c>
+      <c r="Z3" s="1" t="str" cm="1">
+        <f t="array" ref="Z3">INDEX(Z5:Z7,$A$4)</f>
+        <v>IE-RN</v>
+      </c>
+      <c r="AA3" s="1" t="str" cm="1">
+        <f t="array" ref="AA3">INDEX(AA5:AA7,$A$4)</f>
+        <v>IE-SO</v>
+      </c>
+      <c r="AB3" s="1" t="str" cm="1">
+        <f t="array" ref="AB3">INDEX(AB5:AB7,$A$4)</f>
+        <v>IE-CN</v>
+      </c>
+      <c r="AC3" s="1" t="str" cm="1">
+        <f t="array" ref="AC3">INDEX(AC5:AC7,$A$4)</f>
+        <v>IE-DL</v>
+      </c>
+      <c r="AD3" s="1" t="str" cm="1">
+        <f t="array" ref="AD3">INDEX(AD5:AD7,$A$4)</f>
+        <v>IE-MN</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="1" t="str">
+        <f>Regions!A11</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="F5" s="1" t="str">
+        <f>Regions!A16</f>
+        <v>IE-D</v>
+      </c>
+      <c r="G5" s="1" t="str">
+        <f>Regions!A19</f>
+        <v>IE-KE</v>
+      </c>
+      <c r="H5" s="1" t="str">
+        <f>Regions!A20</f>
+        <v>IE-KK</v>
+      </c>
+      <c r="I5" s="1" t="str">
+        <f>Regions!A21</f>
+        <v>IE-LS</v>
+      </c>
+      <c r="J5" s="1" t="str">
+        <f>Regions!A24</f>
+        <v>IE-LD</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f>Regions!A25</f>
+        <v>IE-LH</v>
+      </c>
+      <c r="L5" s="1" t="str">
+        <f>Regions!A27</f>
+        <v>IE-MH</v>
+      </c>
+      <c r="M5" s="1" t="str">
+        <f>Regions!A29</f>
+        <v>IE-OY</v>
+      </c>
+      <c r="N5" s="1" t="str">
+        <f>Regions!A34</f>
+        <v>IE-WH</v>
+      </c>
+      <c r="O5" s="1" t="str">
+        <f>Regions!A35</f>
+        <v>IE-WX</v>
+      </c>
+      <c r="P5" s="1" t="str">
+        <f>Regions!A36</f>
+        <v>IE-WW</v>
+      </c>
+      <c r="Q5" s="1" t="str">
+        <f>Regions!A13</f>
+        <v>IE-CE</v>
+      </c>
+      <c r="R5" s="1" t="str">
+        <f>Regions!A14</f>
+        <v>IE-CO</v>
+      </c>
+      <c r="S5" s="1" t="str">
+        <f>Regions!A18</f>
+        <v>IE-KY</v>
+      </c>
+      <c r="T5" s="1" t="str">
+        <f>Regions!A23</f>
+        <v>IE-LK</v>
+      </c>
+      <c r="U5" s="1" t="str">
+        <f>Regions!A32</f>
+        <v>IE-TA</v>
+      </c>
+      <c r="V5" s="1" t="str">
+        <f>Regions!A33</f>
+        <v>IE-WD</v>
+      </c>
+      <c r="W5" s="1" t="str">
+        <f>Regions!A17</f>
+        <v>IE-G</v>
+      </c>
+      <c r="X5" s="1" t="str">
+        <f>Regions!A22</f>
+        <v>IE-LM</v>
+      </c>
+      <c r="Y5" s="1" t="str">
+        <f>Regions!A26</f>
+        <v>IE-MO</v>
+      </c>
+      <c r="Z5" s="1" t="str">
+        <f>Regions!A30</f>
+        <v>IE-RN</v>
+      </c>
+      <c r="AA5" s="1" t="str">
+        <f>Regions!A31</f>
+        <v>IE-SO</v>
+      </c>
+      <c r="AB5" s="1" t="str">
+        <f>Regions!A12</f>
+        <v>IE-CN</v>
+      </c>
+      <c r="AC5" s="1" t="str">
+        <f>Regions!A15</f>
+        <v>IE-DL</v>
+      </c>
+      <c r="AD5" s="1" t="str">
+        <f>Regions!A28</f>
+        <v>IE-MN</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="1" t="str">
+        <f>C5</f>
+        <v>IE</v>
+      </c>
+      <c r="D6" s="1" t="str">
+        <f>"*"&amp;D5</f>
+        <v>*National</v>
+      </c>
+      <c r="E6" s="1" t="str">
+        <f t="shared" ref="E6:AD6" si="0">"*"&amp;E5</f>
+        <v>*IE-CW</v>
+      </c>
+      <c r="F6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-D</v>
+      </c>
+      <c r="G6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-KE</v>
+      </c>
+      <c r="H6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-KK</v>
+      </c>
+      <c r="I6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LS</v>
+      </c>
+      <c r="J6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LD</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LH</v>
+      </c>
+      <c r="L6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-MH</v>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-OY</v>
+      </c>
+      <c r="N6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-WH</v>
+      </c>
+      <c r="O6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-WX</v>
+      </c>
+      <c r="P6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-WW</v>
+      </c>
+      <c r="Q6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-CE</v>
+      </c>
+      <c r="R6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-CO</v>
+      </c>
+      <c r="S6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-KY</v>
+      </c>
+      <c r="T6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LK</v>
+      </c>
+      <c r="U6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-TA</v>
+      </c>
+      <c r="V6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-WD</v>
+      </c>
+      <c r="W6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-G</v>
+      </c>
+      <c r="X6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-LM</v>
+      </c>
+      <c r="Y6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-MO</v>
+      </c>
+      <c r="Z6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-RN</v>
+      </c>
+      <c r="AA6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-SO</v>
+      </c>
+      <c r="AB6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-CN</v>
+      </c>
+      <c r="AC6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-DL</v>
+      </c>
+      <c r="AD6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>*IE-MN</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="1" t="str">
+        <f>"*"&amp;C5</f>
+        <v>*IE</v>
+      </c>
+      <c r="D7" s="1" t="str">
+        <f>D5</f>
+        <v>National</v>
+      </c>
+      <c r="E7" s="1" t="str">
+        <f t="shared" ref="E7:AD7" si="1">E5</f>
+        <v>IE-CW</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-D</v>
+      </c>
+      <c r="G7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-KE</v>
+      </c>
+      <c r="H7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-KK</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LS</v>
+      </c>
+      <c r="J7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LD</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LH</v>
+      </c>
+      <c r="L7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-MH</v>
+      </c>
+      <c r="M7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-OY</v>
+      </c>
+      <c r="N7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-WH</v>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-WX</v>
+      </c>
+      <c r="P7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-WW</v>
+      </c>
+      <c r="Q7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-CE</v>
+      </c>
+      <c r="R7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-CO</v>
+      </c>
+      <c r="S7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-KY</v>
+      </c>
+      <c r="T7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LK</v>
+      </c>
+      <c r="U7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-TA</v>
+      </c>
+      <c r="V7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-WD</v>
+      </c>
+      <c r="W7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-G</v>
+      </c>
+      <c r="X7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-LM</v>
+      </c>
+      <c r="Y7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-MO</v>
+      </c>
+      <c r="Z7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-RN</v>
+      </c>
+      <c r="AA7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-SO</v>
+      </c>
+      <c r="AB7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-CN</v>
+      </c>
+      <c r="AC7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-DL</v>
+      </c>
+      <c r="AD7" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>IE-MN</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A11" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A12" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A13" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A14" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A15" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
+      <c r="A16" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A24" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="5121" r:id="rId4" name="Drop Down 1">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>1</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>3</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AP3"/>
+  <dimension ref="A1:AQ3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:AH3"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -967,26 +2034,26 @@
     <col min="6" max="6" width="11.53125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="34" width="10.6640625" customWidth="1"/>
-    <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="8.46484375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.53125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.53125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="9" max="35" width="10.6640625" customWidth="1"/>
+    <col min="36" max="36" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.53125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="8.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:43" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" t="s">
         <v>17</v>
       </c>
@@ -1009,131 +2076,135 @@
         <v>18</v>
       </c>
       <c r="I3" t="str">
-        <f>[1]Regions!C2</f>
+        <f>Regions!C$3</f>
+        <v>IE</v>
+      </c>
+      <c r="J3" t="str">
+        <f>Regions!E$3</f>
         <v>IE-CW</v>
       </c>
-      <c r="J3" t="str">
-        <f>[1]Regions!D2</f>
+      <c r="K3" t="str">
+        <f>Regions!F$3</f>
         <v>IE-D</v>
       </c>
-      <c r="K3" t="str">
-        <f>[1]Regions!E2</f>
+      <c r="L3" t="str">
+        <f>Regions!G$3</f>
         <v>IE-KE</v>
       </c>
-      <c r="L3" t="str">
-        <f>[1]Regions!F2</f>
+      <c r="M3" t="str">
+        <f>Regions!H$3</f>
         <v>IE-KK</v>
       </c>
-      <c r="M3" t="str">
-        <f>[1]Regions!G2</f>
+      <c r="N3" t="str">
+        <f>Regions!I$3</f>
         <v>IE-LS</v>
       </c>
-      <c r="N3" t="str">
-        <f>[1]Regions!H2</f>
+      <c r="O3" t="str">
+        <f>Regions!J$3</f>
         <v>IE-LD</v>
       </c>
-      <c r="O3" t="str">
-        <f>[1]Regions!I2</f>
+      <c r="P3" t="str">
+        <f>Regions!K$3</f>
         <v>IE-LH</v>
       </c>
-      <c r="P3" t="str">
-        <f>[1]Regions!J2</f>
+      <c r="Q3" t="str">
+        <f>Regions!L$3</f>
         <v>IE-MH</v>
       </c>
-      <c r="Q3" t="str">
-        <f>[1]Regions!K2</f>
+      <c r="R3" t="str">
+        <f>Regions!M$3</f>
         <v>IE-OY</v>
       </c>
-      <c r="R3" t="str">
-        <f>[1]Regions!L2</f>
+      <c r="S3" t="str">
+        <f>Regions!N$3</f>
         <v>IE-WH</v>
       </c>
-      <c r="S3" t="str">
-        <f>[1]Regions!M2</f>
+      <c r="T3" t="str">
+        <f>Regions!O$3</f>
         <v>IE-WX</v>
       </c>
-      <c r="T3" t="str">
-        <f>[1]Regions!N2</f>
+      <c r="U3" t="str">
+        <f>Regions!P$3</f>
         <v>IE-WW</v>
       </c>
-      <c r="U3" t="str">
-        <f>[1]Regions!O2</f>
+      <c r="V3" t="str">
+        <f>Regions!Q$3</f>
         <v>IE-CE</v>
       </c>
-      <c r="V3" t="str">
-        <f>[1]Regions!P2</f>
+      <c r="W3" t="str">
+        <f>Regions!R$3</f>
         <v>IE-CO</v>
       </c>
-      <c r="W3" t="str">
-        <f>[1]Regions!Q2</f>
+      <c r="X3" t="str">
+        <f>Regions!S$3</f>
         <v>IE-KY</v>
       </c>
-      <c r="X3" t="str">
-        <f>[1]Regions!R2</f>
+      <c r="Y3" t="str">
+        <f>Regions!T$3</f>
         <v>IE-LK</v>
       </c>
-      <c r="Y3" t="str">
-        <f>[1]Regions!S2</f>
+      <c r="Z3" t="str">
+        <f>Regions!U$3</f>
         <v>IE-TA</v>
       </c>
-      <c r="Z3" t="str">
-        <f>[1]Regions!T2</f>
+      <c r="AA3" t="str">
+        <f>Regions!V$3</f>
         <v>IE-WD</v>
       </c>
-      <c r="AA3" t="str">
-        <f>[1]Regions!U2</f>
+      <c r="AB3" t="str">
+        <f>Regions!W$3</f>
         <v>IE-G</v>
       </c>
-      <c r="AB3" t="str">
-        <f>[1]Regions!V2</f>
+      <c r="AC3" t="str">
+        <f>Regions!X$3</f>
         <v>IE-LM</v>
       </c>
-      <c r="AC3" t="str">
-        <f>[1]Regions!W2</f>
+      <c r="AD3" t="str">
+        <f>Regions!Y$3</f>
         <v>IE-MO</v>
       </c>
-      <c r="AD3" t="str">
-        <f>[1]Regions!X2</f>
+      <c r="AE3" t="str">
+        <f>Regions!Z$3</f>
         <v>IE-RN</v>
       </c>
-      <c r="AE3" t="str">
-        <f>[1]Regions!Y2</f>
+      <c r="AF3" t="str">
+        <f>Regions!AA$3</f>
         <v>IE-SO</v>
       </c>
-      <c r="AF3" t="str">
-        <f>[1]Regions!Z2</f>
+      <c r="AG3" t="str">
+        <f>Regions!AB$3</f>
         <v>IE-CN</v>
       </c>
-      <c r="AG3" t="str">
-        <f>[1]Regions!AA2</f>
+      <c r="AH3" t="str">
+        <f>Regions!AC$3</f>
         <v>IE-DL</v>
       </c>
-      <c r="AH3" t="str">
-        <f>[1]Regions!AB2</f>
+      <c r="AI3" t="str">
+        <f>Regions!AD$3</f>
         <v>IE-MN</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>5</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>4</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>19</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>2</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AN3" t="s">
         <v>7</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
         <v>20</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>6</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AQ3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1143,13 +2214,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:AP3"/>
+  <dimension ref="A1:AQ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AH13" sqref="AH13"/>
+    <sheetView topLeftCell="N3" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:AI3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1161,26 +2232,26 @@
     <col min="6" max="6" width="11.53125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="34" width="10.6640625" customWidth="1"/>
-    <col min="35" max="35" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="8.46484375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.53125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="8.53125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="42" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="9" max="35" width="10.6640625" customWidth="1"/>
+    <col min="36" max="36" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="8.46484375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.53125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="8.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:42" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>17</v>
       </c>
@@ -1203,131 +2274,135 @@
         <v>18</v>
       </c>
       <c r="I3" t="str">
-        <f>[1]Regions!C2</f>
+        <f>Regions!C$3</f>
+        <v>IE</v>
+      </c>
+      <c r="J3" t="str">
+        <f>Regions!E$3</f>
         <v>IE-CW</v>
       </c>
-      <c r="J3" t="str">
-        <f>[1]Regions!D2</f>
+      <c r="K3" t="str">
+        <f>Regions!F$3</f>
         <v>IE-D</v>
       </c>
-      <c r="K3" t="str">
-        <f>[1]Regions!E2</f>
+      <c r="L3" t="str">
+        <f>Regions!G$3</f>
         <v>IE-KE</v>
       </c>
-      <c r="L3" t="str">
-        <f>[1]Regions!F2</f>
+      <c r="M3" t="str">
+        <f>Regions!H$3</f>
         <v>IE-KK</v>
       </c>
-      <c r="M3" t="str">
-        <f>[1]Regions!G2</f>
+      <c r="N3" t="str">
+        <f>Regions!I$3</f>
         <v>IE-LS</v>
       </c>
-      <c r="N3" t="str">
-        <f>[1]Regions!H2</f>
+      <c r="O3" t="str">
+        <f>Regions!J$3</f>
         <v>IE-LD</v>
       </c>
-      <c r="O3" t="str">
-        <f>[1]Regions!I2</f>
+      <c r="P3" t="str">
+        <f>Regions!K$3</f>
         <v>IE-LH</v>
       </c>
-      <c r="P3" t="str">
-        <f>[1]Regions!J2</f>
+      <c r="Q3" t="str">
+        <f>Regions!L$3</f>
         <v>IE-MH</v>
       </c>
-      <c r="Q3" t="str">
-        <f>[1]Regions!K2</f>
+      <c r="R3" t="str">
+        <f>Regions!M$3</f>
         <v>IE-OY</v>
       </c>
-      <c r="R3" t="str">
-        <f>[1]Regions!L2</f>
+      <c r="S3" t="str">
+        <f>Regions!N$3</f>
         <v>IE-WH</v>
       </c>
-      <c r="S3" t="str">
-        <f>[1]Regions!M2</f>
+      <c r="T3" t="str">
+        <f>Regions!O$3</f>
         <v>IE-WX</v>
       </c>
-      <c r="T3" t="str">
-        <f>[1]Regions!N2</f>
+      <c r="U3" t="str">
+        <f>Regions!P$3</f>
         <v>IE-WW</v>
       </c>
-      <c r="U3" t="str">
-        <f>[1]Regions!O2</f>
+      <c r="V3" t="str">
+        <f>Regions!Q$3</f>
         <v>IE-CE</v>
       </c>
-      <c r="V3" t="str">
-        <f>[1]Regions!P2</f>
+      <c r="W3" t="str">
+        <f>Regions!R$3</f>
         <v>IE-CO</v>
       </c>
-      <c r="W3" t="str">
-        <f>[1]Regions!Q2</f>
+      <c r="X3" t="str">
+        <f>Regions!S$3</f>
         <v>IE-KY</v>
       </c>
-      <c r="X3" t="str">
-        <f>[1]Regions!R2</f>
+      <c r="Y3" t="str">
+        <f>Regions!T$3</f>
         <v>IE-LK</v>
       </c>
-      <c r="Y3" t="str">
-        <f>[1]Regions!S2</f>
+      <c r="Z3" t="str">
+        <f>Regions!U$3</f>
         <v>IE-TA</v>
       </c>
-      <c r="Z3" t="str">
-        <f>[1]Regions!T2</f>
+      <c r="AA3" t="str">
+        <f>Regions!V$3</f>
         <v>IE-WD</v>
       </c>
-      <c r="AA3" t="str">
-        <f>[1]Regions!U2</f>
+      <c r="AB3" t="str">
+        <f>Regions!W$3</f>
         <v>IE-G</v>
       </c>
-      <c r="AB3" t="str">
-        <f>[1]Regions!V2</f>
+      <c r="AC3" t="str">
+        <f>Regions!X$3</f>
         <v>IE-LM</v>
       </c>
-      <c r="AC3" t="str">
-        <f>[1]Regions!W2</f>
+      <c r="AD3" t="str">
+        <f>Regions!Y$3</f>
         <v>IE-MO</v>
       </c>
-      <c r="AD3" t="str">
-        <f>[1]Regions!X2</f>
+      <c r="AE3" t="str">
+        <f>Regions!Z$3</f>
         <v>IE-RN</v>
       </c>
-      <c r="AE3" t="str">
-        <f>[1]Regions!Y2</f>
+      <c r="AF3" t="str">
+        <f>Regions!AA$3</f>
         <v>IE-SO</v>
       </c>
-      <c r="AF3" t="str">
-        <f>[1]Regions!Z2</f>
+      <c r="AG3" t="str">
+        <f>Regions!AB$3</f>
         <v>IE-CN</v>
       </c>
-      <c r="AG3" t="str">
-        <f>[1]Regions!AA2</f>
+      <c r="AH3" t="str">
+        <f>Regions!AC$3</f>
         <v>IE-DL</v>
       </c>
-      <c r="AH3" t="str">
-        <f>[1]Regions!AB2</f>
+      <c r="AI3" t="str">
+        <f>Regions!AD$3</f>
         <v>IE-MN</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AJ3" t="s">
         <v>5</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AK3" t="s">
         <v>4</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AL3" t="s">
         <v>19</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AM3" t="s">
         <v>2</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AN3" t="s">
         <v>7</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AO3" t="s">
         <v>20</v>
       </c>
-      <c r="AO3" t="s">
+      <c r="AP3" t="s">
         <v>6</v>
       </c>
-      <c r="AP3" t="s">
+      <c r="AQ3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1337,7 +2412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:O5"/>
@@ -1420,7 +2495,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O5"/>
@@ -1503,7 +2578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:O5"/>
@@ -1586,7 +2661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:O5"/>
@@ -1668,13 +2743,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="B3:AG54"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T54" sqref="T54"/>
+      <selection activeCell="G4" sqref="G4:AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1687,7 +2762,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:33" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="2:33" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -1704,111 +2779,111 @@
         <v>3</v>
       </c>
       <c r="G4" t="str">
-        <f>[1]Regions!B2</f>
-        <v>*National</v>
+        <f>Regions!C$3</f>
+        <v>IE</v>
       </c>
       <c r="H4" t="str">
-        <f>[1]Regions!C2</f>
+        <f>Regions!E$3</f>
         <v>IE-CW</v>
       </c>
       <c r="I4" t="str">
-        <f>[1]Regions!D2</f>
+        <f>Regions!F$3</f>
         <v>IE-D</v>
       </c>
       <c r="J4" t="str">
-        <f>[1]Regions!E2</f>
+        <f>Regions!G$3</f>
         <v>IE-KE</v>
       </c>
       <c r="K4" t="str">
-        <f>[1]Regions!F2</f>
+        <f>Regions!H$3</f>
         <v>IE-KK</v>
       </c>
       <c r="L4" t="str">
-        <f>[1]Regions!G2</f>
+        <f>Regions!I$3</f>
         <v>IE-LS</v>
       </c>
       <c r="M4" t="str">
-        <f>[1]Regions!H2</f>
+        <f>Regions!J$3</f>
         <v>IE-LD</v>
       </c>
       <c r="N4" t="str">
-        <f>[1]Regions!I2</f>
+        <f>Regions!K$3</f>
         <v>IE-LH</v>
       </c>
       <c r="O4" t="str">
-        <f>[1]Regions!J2</f>
+        <f>Regions!L$3</f>
         <v>IE-MH</v>
       </c>
       <c r="P4" t="str">
-        <f>[1]Regions!K2</f>
+        <f>Regions!M$3</f>
         <v>IE-OY</v>
       </c>
       <c r="Q4" t="str">
-        <f>[1]Regions!L2</f>
+        <f>Regions!N$3</f>
         <v>IE-WH</v>
       </c>
       <c r="R4" t="str">
-        <f>[1]Regions!M2</f>
+        <f>Regions!O$3</f>
         <v>IE-WX</v>
       </c>
       <c r="S4" t="str">
-        <f>[1]Regions!N2</f>
+        <f>Regions!P$3</f>
         <v>IE-WW</v>
       </c>
       <c r="T4" t="str">
-        <f>[1]Regions!O2</f>
+        <f>Regions!Q$3</f>
         <v>IE-CE</v>
       </c>
       <c r="U4" t="str">
-        <f>[1]Regions!P2</f>
+        <f>Regions!R$3</f>
         <v>IE-CO</v>
       </c>
       <c r="V4" t="str">
-        <f>[1]Regions!Q2</f>
+        <f>Regions!S$3</f>
         <v>IE-KY</v>
       </c>
       <c r="W4" t="str">
-        <f>[1]Regions!R2</f>
+        <f>Regions!T$3</f>
         <v>IE-LK</v>
       </c>
       <c r="X4" t="str">
-        <f>[1]Regions!S2</f>
+        <f>Regions!U$3</f>
         <v>IE-TA</v>
       </c>
       <c r="Y4" t="str">
-        <f>[1]Regions!T2</f>
+        <f>Regions!V$3</f>
         <v>IE-WD</v>
       </c>
       <c r="Z4" t="str">
-        <f>[1]Regions!U2</f>
+        <f>Regions!W$3</f>
         <v>IE-G</v>
       </c>
       <c r="AA4" t="str">
-        <f>[1]Regions!V2</f>
+        <f>Regions!X$3</f>
         <v>IE-LM</v>
       </c>
       <c r="AB4" t="str">
-        <f>[1]Regions!W2</f>
+        <f>Regions!Y$3</f>
         <v>IE-MO</v>
       </c>
       <c r="AC4" t="str">
-        <f>[1]Regions!X2</f>
+        <f>Regions!Z$3</f>
         <v>IE-RN</v>
       </c>
       <c r="AD4" t="str">
-        <f>[1]Regions!Y2</f>
+        <f>Regions!AA$3</f>
         <v>IE-SO</v>
       </c>
       <c r="AE4" t="str">
-        <f>[1]Regions!Z2</f>
+        <f>Regions!AB$3</f>
         <v>IE-CN</v>
       </c>
       <c r="AF4" t="str">
-        <f>[1]Regions!AA2</f>
+        <f>Regions!AC$3</f>
         <v>IE-DL</v>
       </c>
       <c r="AG4" t="str">
-        <f>[1]Regions!AB2</f>
+        <f>Regions!AD$3</f>
         <v>IE-MN</v>
       </c>
     </row>

</xml_diff>